<commit_message>
prompt D added with a traffic accident example
</commit_message>
<xml_diff>
--- a/app/datasets/traffic_accident_reports_collection.xlsx
+++ b/app/datasets/traffic_accident_reports_collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Documents\Proyectos\DS-Projects\VSprojects\reportingAgent\app\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD94865F-368F-4733-B7FA-2DECC619C4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F33FB-D360-480D-A20E-5BC60FD02E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-6096" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRAFFIC_ACCIDENT" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="1008">
   <si>
     <t>report_name</t>
   </si>
@@ -3057,30 +3057,6 @@
   </si>
   <si>
     <t>Automatically generated in batches of size 10 - gpt-4.101</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.601</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.602</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.603</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.604</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.605</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.606</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.607</t>
-  </si>
-  <si>
-    <t>Automatically generated in batches of size 10 - gpt-4.608</t>
   </si>
 </sst>
 </file>
@@ -3153,7 +3129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3163,6 +3139,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3466,10 +3445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K609"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3517,7 +3496,7 @@
       <c r="A2" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>738</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -7147,1575 +7126,6 @@
       </c>
       <c r="K102" s="1" t="s">
         <v>1007</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K103" s="1"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K104" s="1"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K105" s="1"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K106" s="1"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K107" s="1"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K108" s="1"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K109" s="1"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K110" s="1"/>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K111" s="1"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K112" s="1"/>
-    </row>
-    <row r="113" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K113" s="1"/>
-    </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K114" s="1"/>
-    </row>
-    <row r="115" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K115" s="1"/>
-    </row>
-    <row r="116" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K116" s="1"/>
-    </row>
-    <row r="117" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K117" s="1"/>
-    </row>
-    <row r="118" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K118" s="1"/>
-    </row>
-    <row r="119" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K119" s="1"/>
-    </row>
-    <row r="120" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K120" s="1"/>
-    </row>
-    <row r="121" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K121" s="1"/>
-    </row>
-    <row r="122" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K122" s="1"/>
-    </row>
-    <row r="123" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K123" s="1"/>
-    </row>
-    <row r="124" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K124" s="1"/>
-    </row>
-    <row r="125" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K125" s="1"/>
-    </row>
-    <row r="126" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K126" s="1"/>
-    </row>
-    <row r="127" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K127" s="1"/>
-    </row>
-    <row r="128" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K128" s="1"/>
-    </row>
-    <row r="129" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K129" s="1"/>
-    </row>
-    <row r="130" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K130" s="1"/>
-    </row>
-    <row r="131" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K131" s="1"/>
-    </row>
-    <row r="132" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K132" s="1"/>
-    </row>
-    <row r="133" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K133" s="1"/>
-    </row>
-    <row r="134" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K134" s="1"/>
-    </row>
-    <row r="135" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K135" s="1"/>
-    </row>
-    <row r="136" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K136" s="1"/>
-    </row>
-    <row r="137" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K137" s="1"/>
-    </row>
-    <row r="138" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K138" s="1"/>
-    </row>
-    <row r="139" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K139" s="1"/>
-    </row>
-    <row r="140" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K140" s="1"/>
-    </row>
-    <row r="141" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K141" s="1"/>
-    </row>
-    <row r="142" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K142" s="1"/>
-    </row>
-    <row r="143" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K143" s="1"/>
-    </row>
-    <row r="144" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K144" s="1"/>
-    </row>
-    <row r="145" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K145" s="1"/>
-    </row>
-    <row r="146" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K146" s="1"/>
-    </row>
-    <row r="147" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K147" s="1"/>
-    </row>
-    <row r="148" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K148" s="1"/>
-    </row>
-    <row r="149" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K149" s="1"/>
-    </row>
-    <row r="150" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K150" s="1"/>
-    </row>
-    <row r="151" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K151" s="1"/>
-    </row>
-    <row r="152" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K152" s="1"/>
-    </row>
-    <row r="153" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K153" s="1"/>
-    </row>
-    <row r="154" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K154" s="1"/>
-    </row>
-    <row r="155" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K155" s="1"/>
-    </row>
-    <row r="156" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K156" s="1"/>
-    </row>
-    <row r="157" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K157" s="1"/>
-    </row>
-    <row r="158" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K158" s="1"/>
-    </row>
-    <row r="159" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K159" s="1"/>
-    </row>
-    <row r="160" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K160" s="1"/>
-    </row>
-    <row r="161" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K161" s="1"/>
-    </row>
-    <row r="162" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K162" s="1"/>
-    </row>
-    <row r="163" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K163" s="1"/>
-    </row>
-    <row r="164" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K164" s="1"/>
-    </row>
-    <row r="165" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K165" s="1"/>
-    </row>
-    <row r="166" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K166" s="1"/>
-    </row>
-    <row r="167" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K167" s="1"/>
-    </row>
-    <row r="168" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K168" s="1"/>
-    </row>
-    <row r="169" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K169" s="1"/>
-    </row>
-    <row r="170" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K170" s="1"/>
-    </row>
-    <row r="171" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K171" s="1"/>
-    </row>
-    <row r="172" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K172" s="1"/>
-    </row>
-    <row r="173" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K173" s="1"/>
-    </row>
-    <row r="174" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K174" s="1"/>
-    </row>
-    <row r="175" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K175" s="1"/>
-    </row>
-    <row r="176" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K176" s="1"/>
-    </row>
-    <row r="177" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K177" s="1"/>
-    </row>
-    <row r="178" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K178" s="1"/>
-    </row>
-    <row r="179" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K179" s="1"/>
-    </row>
-    <row r="180" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K180" s="1"/>
-    </row>
-    <row r="181" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K181" s="1"/>
-    </row>
-    <row r="182" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K182" s="1"/>
-    </row>
-    <row r="183" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K183" s="1"/>
-    </row>
-    <row r="184" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K184" s="1"/>
-    </row>
-    <row r="185" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K185" s="1"/>
-    </row>
-    <row r="186" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K186" s="1"/>
-    </row>
-    <row r="187" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K187" s="1"/>
-    </row>
-    <row r="188" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K188" s="1"/>
-    </row>
-    <row r="189" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K189" s="1"/>
-    </row>
-    <row r="190" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K190" s="1"/>
-    </row>
-    <row r="191" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K191" s="1"/>
-    </row>
-    <row r="192" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K192" s="1"/>
-    </row>
-    <row r="193" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K193" s="1"/>
-    </row>
-    <row r="194" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K194" s="1"/>
-    </row>
-    <row r="195" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K195" s="1"/>
-    </row>
-    <row r="196" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K196" s="1"/>
-    </row>
-    <row r="197" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K197" s="1"/>
-    </row>
-    <row r="198" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K198" s="1"/>
-    </row>
-    <row r="199" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K199" s="1"/>
-    </row>
-    <row r="200" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K200" s="1"/>
-    </row>
-    <row r="201" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K201" s="1"/>
-    </row>
-    <row r="202" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K202" s="1"/>
-    </row>
-    <row r="203" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K203" s="1"/>
-    </row>
-    <row r="204" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K204" s="1"/>
-    </row>
-    <row r="205" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K205" s="1"/>
-    </row>
-    <row r="206" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K206" s="1"/>
-    </row>
-    <row r="207" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K207" s="1"/>
-    </row>
-    <row r="208" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K208" s="1"/>
-    </row>
-    <row r="209" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K209" s="1"/>
-    </row>
-    <row r="210" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K210" s="1"/>
-    </row>
-    <row r="211" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K211" s="1"/>
-    </row>
-    <row r="212" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K212" s="1"/>
-    </row>
-    <row r="213" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K213" s="1"/>
-    </row>
-    <row r="214" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K214" s="1"/>
-    </row>
-    <row r="215" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K215" s="1"/>
-    </row>
-    <row r="216" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K216" s="1"/>
-    </row>
-    <row r="217" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K217" s="1"/>
-    </row>
-    <row r="218" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K218" s="1"/>
-    </row>
-    <row r="219" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K219" s="1"/>
-    </row>
-    <row r="220" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K220" s="1"/>
-    </row>
-    <row r="221" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K221" s="1"/>
-    </row>
-    <row r="222" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K222" s="1"/>
-    </row>
-    <row r="223" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K223" s="1"/>
-    </row>
-    <row r="224" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K224" s="1"/>
-    </row>
-    <row r="225" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K225" s="1"/>
-    </row>
-    <row r="226" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K226" s="1"/>
-    </row>
-    <row r="227" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K227" s="1"/>
-    </row>
-    <row r="228" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K228" s="1"/>
-    </row>
-    <row r="229" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K229" s="1"/>
-    </row>
-    <row r="230" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K230" s="1"/>
-    </row>
-    <row r="231" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K231" s="1"/>
-    </row>
-    <row r="232" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K232" s="1"/>
-    </row>
-    <row r="233" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K233" s="1"/>
-    </row>
-    <row r="234" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K234" s="1"/>
-    </row>
-    <row r="235" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K235" s="1"/>
-    </row>
-    <row r="236" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K236" s="1"/>
-    </row>
-    <row r="237" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K237" s="1"/>
-    </row>
-    <row r="238" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K238" s="1"/>
-    </row>
-    <row r="239" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K239" s="1"/>
-    </row>
-    <row r="240" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K240" s="1"/>
-    </row>
-    <row r="241" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K241" s="1"/>
-    </row>
-    <row r="242" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K242" s="1"/>
-    </row>
-    <row r="243" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K243" s="1"/>
-    </row>
-    <row r="244" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K244" s="1"/>
-    </row>
-    <row r="245" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K245" s="1"/>
-    </row>
-    <row r="246" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K246" s="1"/>
-    </row>
-    <row r="247" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K247" s="1"/>
-    </row>
-    <row r="248" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K248" s="1"/>
-    </row>
-    <row r="249" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K249" s="1"/>
-    </row>
-    <row r="250" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K250" s="1"/>
-    </row>
-    <row r="251" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K251" s="1"/>
-    </row>
-    <row r="252" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K252" s="1"/>
-    </row>
-    <row r="253" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K253" s="1"/>
-    </row>
-    <row r="254" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K254" s="1"/>
-    </row>
-    <row r="255" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K255" s="1"/>
-    </row>
-    <row r="256" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K256" s="1"/>
-    </row>
-    <row r="257" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K257" s="1"/>
-    </row>
-    <row r="258" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K258" s="1"/>
-    </row>
-    <row r="259" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K259" s="1"/>
-    </row>
-    <row r="260" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K260" s="1"/>
-    </row>
-    <row r="261" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K261" s="1"/>
-    </row>
-    <row r="262" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K262" s="1"/>
-    </row>
-    <row r="263" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K263" s="1"/>
-    </row>
-    <row r="264" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K264" s="1"/>
-    </row>
-    <row r="265" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K265" s="1"/>
-    </row>
-    <row r="266" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K266" s="1"/>
-    </row>
-    <row r="267" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K267" s="1"/>
-    </row>
-    <row r="268" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K268" s="1"/>
-    </row>
-    <row r="269" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K269" s="1"/>
-    </row>
-    <row r="270" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K270" s="1"/>
-    </row>
-    <row r="271" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K271" s="1"/>
-    </row>
-    <row r="272" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K272" s="1"/>
-    </row>
-    <row r="273" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K273" s="1"/>
-    </row>
-    <row r="274" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K274" s="1"/>
-    </row>
-    <row r="275" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K275" s="1"/>
-    </row>
-    <row r="276" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K276" s="1"/>
-    </row>
-    <row r="277" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K277" s="1"/>
-    </row>
-    <row r="278" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K278" s="1"/>
-    </row>
-    <row r="279" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K279" s="1"/>
-    </row>
-    <row r="280" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K280" s="1"/>
-    </row>
-    <row r="281" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K281" s="1"/>
-    </row>
-    <row r="282" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K282" s="1"/>
-    </row>
-    <row r="283" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K283" s="1"/>
-    </row>
-    <row r="284" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K284" s="1"/>
-    </row>
-    <row r="285" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K285" s="1"/>
-    </row>
-    <row r="286" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K286" s="1"/>
-    </row>
-    <row r="287" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K287" s="1"/>
-    </row>
-    <row r="288" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K288" s="1"/>
-    </row>
-    <row r="289" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K289" s="1"/>
-    </row>
-    <row r="290" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K290" s="1"/>
-    </row>
-    <row r="291" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K291" s="1"/>
-    </row>
-    <row r="292" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K292" s="1"/>
-    </row>
-    <row r="293" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K293" s="1"/>
-    </row>
-    <row r="294" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K294" s="1"/>
-    </row>
-    <row r="295" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K295" s="1"/>
-    </row>
-    <row r="296" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K296" s="1"/>
-    </row>
-    <row r="297" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K297" s="1"/>
-    </row>
-    <row r="298" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K298" s="1"/>
-    </row>
-    <row r="299" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K299" s="1"/>
-    </row>
-    <row r="300" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K300" s="1"/>
-    </row>
-    <row r="301" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K301" s="1"/>
-    </row>
-    <row r="302" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K302" s="1"/>
-    </row>
-    <row r="303" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K303" s="1"/>
-    </row>
-    <row r="304" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K304" s="1"/>
-    </row>
-    <row r="305" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K305" s="1"/>
-    </row>
-    <row r="306" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K306" s="1"/>
-    </row>
-    <row r="307" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K307" s="1"/>
-    </row>
-    <row r="308" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K308" s="1"/>
-    </row>
-    <row r="309" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K309" s="1"/>
-    </row>
-    <row r="310" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K310" s="1"/>
-    </row>
-    <row r="311" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K311" s="1"/>
-    </row>
-    <row r="312" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K312" s="1"/>
-    </row>
-    <row r="313" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K313" s="1"/>
-    </row>
-    <row r="314" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K314" s="1"/>
-    </row>
-    <row r="315" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K315" s="1"/>
-    </row>
-    <row r="316" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K316" s="1"/>
-    </row>
-    <row r="317" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K317" s="1"/>
-    </row>
-    <row r="318" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K318" s="1"/>
-    </row>
-    <row r="319" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K319" s="1"/>
-    </row>
-    <row r="320" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K320" s="1"/>
-    </row>
-    <row r="321" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K321" s="1"/>
-    </row>
-    <row r="322" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K322" s="1"/>
-    </row>
-    <row r="323" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K323" s="1"/>
-    </row>
-    <row r="324" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K324" s="1"/>
-    </row>
-    <row r="325" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K325" s="1"/>
-    </row>
-    <row r="326" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K326" s="1"/>
-    </row>
-    <row r="327" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K327" s="1"/>
-    </row>
-    <row r="328" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K328" s="1"/>
-    </row>
-    <row r="329" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K329" s="1"/>
-    </row>
-    <row r="330" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K330" s="1"/>
-    </row>
-    <row r="331" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K331" s="1"/>
-    </row>
-    <row r="332" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K332" s="1"/>
-    </row>
-    <row r="333" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K333" s="1"/>
-    </row>
-    <row r="334" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K334" s="1"/>
-    </row>
-    <row r="335" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K335" s="1"/>
-    </row>
-    <row r="336" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K336" s="1"/>
-    </row>
-    <row r="337" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K337" s="1"/>
-    </row>
-    <row r="338" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K338" s="1"/>
-    </row>
-    <row r="339" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K339" s="1"/>
-    </row>
-    <row r="340" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K340" s="1"/>
-    </row>
-    <row r="341" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K341" s="1"/>
-    </row>
-    <row r="342" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K342" s="1"/>
-    </row>
-    <row r="343" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K343" s="1"/>
-    </row>
-    <row r="344" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K344" s="1"/>
-    </row>
-    <row r="345" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K345" s="1"/>
-    </row>
-    <row r="346" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K346" s="1"/>
-    </row>
-    <row r="347" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K347" s="1"/>
-    </row>
-    <row r="348" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K348" s="1"/>
-    </row>
-    <row r="349" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K349" s="1"/>
-    </row>
-    <row r="350" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K350" s="1"/>
-    </row>
-    <row r="351" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K351" s="1"/>
-    </row>
-    <row r="352" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K352" s="1"/>
-    </row>
-    <row r="353" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K353" s="1"/>
-    </row>
-    <row r="354" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K354" s="1"/>
-    </row>
-    <row r="355" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K355" s="1"/>
-    </row>
-    <row r="356" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K356" s="1"/>
-    </row>
-    <row r="357" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K357" s="1"/>
-    </row>
-    <row r="358" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K358" s="1"/>
-    </row>
-    <row r="359" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K359" s="1"/>
-    </row>
-    <row r="360" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K360" s="1"/>
-    </row>
-    <row r="361" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K361" s="1"/>
-    </row>
-    <row r="362" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K362" s="1"/>
-    </row>
-    <row r="363" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K363" s="1"/>
-    </row>
-    <row r="364" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K364" s="1"/>
-    </row>
-    <row r="365" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K365" s="1"/>
-    </row>
-    <row r="366" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K366" s="1"/>
-    </row>
-    <row r="367" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K367" s="1"/>
-    </row>
-    <row r="368" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K368" s="1"/>
-    </row>
-    <row r="369" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K369" s="1"/>
-    </row>
-    <row r="370" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K370" s="1"/>
-    </row>
-    <row r="371" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K371" s="1"/>
-    </row>
-    <row r="372" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K372" s="1"/>
-    </row>
-    <row r="373" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K373" s="1"/>
-    </row>
-    <row r="374" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K374" s="1"/>
-    </row>
-    <row r="375" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K375" s="1"/>
-    </row>
-    <row r="376" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K376" s="1"/>
-    </row>
-    <row r="377" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K377" s="1"/>
-    </row>
-    <row r="378" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K378" s="1"/>
-    </row>
-    <row r="379" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K379" s="1"/>
-    </row>
-    <row r="380" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K380" s="1"/>
-    </row>
-    <row r="381" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K381" s="1"/>
-    </row>
-    <row r="382" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K382" s="1"/>
-    </row>
-    <row r="383" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K383" s="1"/>
-    </row>
-    <row r="384" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K384" s="1"/>
-    </row>
-    <row r="385" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K385" s="1"/>
-    </row>
-    <row r="386" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K386" s="1"/>
-    </row>
-    <row r="387" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K387" s="1"/>
-    </row>
-    <row r="388" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K388" s="1"/>
-    </row>
-    <row r="389" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K389" s="1"/>
-    </row>
-    <row r="390" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K390" s="1"/>
-    </row>
-    <row r="391" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K391" s="1"/>
-    </row>
-    <row r="392" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K392" s="1"/>
-    </row>
-    <row r="393" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K393" s="1"/>
-    </row>
-    <row r="394" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K394" s="1"/>
-    </row>
-    <row r="395" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K395" s="1"/>
-    </row>
-    <row r="396" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K396" s="1"/>
-    </row>
-    <row r="397" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K397" s="1"/>
-    </row>
-    <row r="398" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K398" s="1"/>
-    </row>
-    <row r="399" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K399" s="1"/>
-    </row>
-    <row r="400" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K400" s="1"/>
-    </row>
-    <row r="401" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K401" s="1"/>
-    </row>
-    <row r="402" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K402" s="1"/>
-    </row>
-    <row r="403" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K403" s="1"/>
-    </row>
-    <row r="404" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K404" s="1"/>
-    </row>
-    <row r="405" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K405" s="1"/>
-    </row>
-    <row r="406" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K406" s="1"/>
-    </row>
-    <row r="407" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K407" s="1"/>
-    </row>
-    <row r="408" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K408" s="1"/>
-    </row>
-    <row r="409" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K409" s="1"/>
-    </row>
-    <row r="410" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K410" s="1"/>
-    </row>
-    <row r="411" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K411" s="1"/>
-    </row>
-    <row r="412" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K412" s="1"/>
-    </row>
-    <row r="413" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K413" s="1"/>
-    </row>
-    <row r="414" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K414" s="1"/>
-    </row>
-    <row r="415" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K415" s="1"/>
-    </row>
-    <row r="416" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K416" s="1"/>
-    </row>
-    <row r="417" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K417" s="1"/>
-    </row>
-    <row r="418" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K418" s="1"/>
-    </row>
-    <row r="419" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K419" s="1"/>
-    </row>
-    <row r="420" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K420" s="1"/>
-    </row>
-    <row r="421" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K421" s="1"/>
-    </row>
-    <row r="422" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K422" s="1"/>
-    </row>
-    <row r="423" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K423" s="1"/>
-    </row>
-    <row r="424" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K424" s="1"/>
-    </row>
-    <row r="425" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K425" s="1"/>
-    </row>
-    <row r="426" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K426" s="1"/>
-    </row>
-    <row r="427" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K427" s="1"/>
-    </row>
-    <row r="428" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K428" s="1"/>
-    </row>
-    <row r="429" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K429" s="1"/>
-    </row>
-    <row r="430" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K430" s="1"/>
-    </row>
-    <row r="431" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K431" s="1"/>
-    </row>
-    <row r="432" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K432" s="1"/>
-    </row>
-    <row r="433" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K433" s="1"/>
-    </row>
-    <row r="434" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K434" s="1"/>
-    </row>
-    <row r="435" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K435" s="1"/>
-    </row>
-    <row r="436" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K436" s="1"/>
-    </row>
-    <row r="437" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K437" s="1"/>
-    </row>
-    <row r="438" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K438" s="1"/>
-    </row>
-    <row r="439" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K439" s="1"/>
-    </row>
-    <row r="440" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K440" s="1"/>
-    </row>
-    <row r="441" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K441" s="1"/>
-    </row>
-    <row r="442" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K442" s="1"/>
-    </row>
-    <row r="443" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K443" s="1"/>
-    </row>
-    <row r="444" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K444" s="1"/>
-    </row>
-    <row r="445" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K445" s="1"/>
-    </row>
-    <row r="446" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K446" s="1"/>
-    </row>
-    <row r="447" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K447" s="1"/>
-    </row>
-    <row r="448" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K448" s="1"/>
-    </row>
-    <row r="449" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K449" s="1"/>
-    </row>
-    <row r="450" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K450" s="1"/>
-    </row>
-    <row r="451" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K451" s="1"/>
-    </row>
-    <row r="452" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K452" s="1"/>
-    </row>
-    <row r="453" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K453" s="1"/>
-    </row>
-    <row r="454" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K454" s="1"/>
-    </row>
-    <row r="455" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K455" s="1"/>
-    </row>
-    <row r="456" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K456" s="1"/>
-    </row>
-    <row r="457" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K457" s="1"/>
-    </row>
-    <row r="458" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K458" s="1"/>
-    </row>
-    <row r="459" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K459" s="1"/>
-    </row>
-    <row r="460" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K460" s="1"/>
-    </row>
-    <row r="461" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K461" s="1"/>
-    </row>
-    <row r="462" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K462" s="1"/>
-    </row>
-    <row r="463" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K463" s="1"/>
-    </row>
-    <row r="464" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K464" s="1"/>
-    </row>
-    <row r="465" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K465" s="1"/>
-    </row>
-    <row r="466" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K466" s="1"/>
-    </row>
-    <row r="467" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K467" s="1"/>
-    </row>
-    <row r="468" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K468" s="1"/>
-    </row>
-    <row r="469" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K469" s="1"/>
-    </row>
-    <row r="470" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K470" s="1"/>
-    </row>
-    <row r="471" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K471" s="1"/>
-    </row>
-    <row r="472" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K472" s="1"/>
-    </row>
-    <row r="473" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K473" s="1"/>
-    </row>
-    <row r="474" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K474" s="1"/>
-    </row>
-    <row r="475" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K475" s="1"/>
-    </row>
-    <row r="476" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K476" s="1"/>
-    </row>
-    <row r="477" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K477" s="1"/>
-    </row>
-    <row r="478" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K478" s="1"/>
-    </row>
-    <row r="479" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K479" s="1"/>
-    </row>
-    <row r="480" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K480" s="1"/>
-    </row>
-    <row r="481" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K481" s="1"/>
-    </row>
-    <row r="482" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K482" s="1"/>
-    </row>
-    <row r="483" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K483" s="1"/>
-    </row>
-    <row r="484" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K484" s="1"/>
-    </row>
-    <row r="485" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K485" s="1"/>
-    </row>
-    <row r="486" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K486" s="1"/>
-    </row>
-    <row r="487" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K487" s="1"/>
-    </row>
-    <row r="488" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K488" s="1"/>
-    </row>
-    <row r="489" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K489" s="1"/>
-    </row>
-    <row r="490" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K490" s="1"/>
-    </row>
-    <row r="491" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K491" s="1"/>
-    </row>
-    <row r="492" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K492" s="1"/>
-    </row>
-    <row r="493" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K493" s="1"/>
-    </row>
-    <row r="494" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K494" s="1"/>
-    </row>
-    <row r="495" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K495" s="1"/>
-    </row>
-    <row r="496" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K496" s="1"/>
-    </row>
-    <row r="497" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K497" s="1"/>
-    </row>
-    <row r="498" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K498" s="1"/>
-    </row>
-    <row r="499" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K499" s="1"/>
-    </row>
-    <row r="500" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K500" s="1"/>
-    </row>
-    <row r="501" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K501" s="1"/>
-    </row>
-    <row r="502" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K502" s="1"/>
-    </row>
-    <row r="503" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K503" s="1"/>
-    </row>
-    <row r="504" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K504" s="1"/>
-    </row>
-    <row r="505" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K505" s="1"/>
-    </row>
-    <row r="506" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K506" s="1"/>
-    </row>
-    <row r="507" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K507" s="1"/>
-    </row>
-    <row r="508" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K508" s="1"/>
-    </row>
-    <row r="509" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K509" s="1"/>
-    </row>
-    <row r="510" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K510" s="1"/>
-    </row>
-    <row r="511" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K511" s="1"/>
-    </row>
-    <row r="512" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K512" s="1"/>
-    </row>
-    <row r="513" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K513" s="1"/>
-    </row>
-    <row r="514" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K514" s="1"/>
-    </row>
-    <row r="515" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K515" s="1"/>
-    </row>
-    <row r="516" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K516" s="1"/>
-    </row>
-    <row r="517" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K517" s="1"/>
-    </row>
-    <row r="518" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K518" s="1"/>
-    </row>
-    <row r="519" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K519" s="1"/>
-    </row>
-    <row r="520" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K520" s="1"/>
-    </row>
-    <row r="521" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K521" s="1"/>
-    </row>
-    <row r="522" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K522" s="1"/>
-    </row>
-    <row r="523" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K523" s="1"/>
-    </row>
-    <row r="524" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K524" s="1"/>
-    </row>
-    <row r="525" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K525" s="1"/>
-    </row>
-    <row r="526" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K526" s="1"/>
-    </row>
-    <row r="527" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K527" s="1"/>
-    </row>
-    <row r="528" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K528" s="1"/>
-    </row>
-    <row r="529" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K529" s="1"/>
-    </row>
-    <row r="530" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K530" s="1"/>
-    </row>
-    <row r="531" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K531" s="1"/>
-    </row>
-    <row r="532" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K532" s="1"/>
-    </row>
-    <row r="533" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K533" s="1"/>
-    </row>
-    <row r="534" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K534" s="1"/>
-    </row>
-    <row r="535" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K535" s="1"/>
-    </row>
-    <row r="536" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K536" s="1"/>
-    </row>
-    <row r="537" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K537" s="1"/>
-    </row>
-    <row r="538" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K538" s="1"/>
-    </row>
-    <row r="539" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K539" s="1"/>
-    </row>
-    <row r="540" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K540" s="1"/>
-    </row>
-    <row r="541" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K541" s="1"/>
-    </row>
-    <row r="542" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K542" s="1"/>
-    </row>
-    <row r="543" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K543" s="1"/>
-    </row>
-    <row r="544" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K544" s="1"/>
-    </row>
-    <row r="545" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K545" s="1"/>
-    </row>
-    <row r="546" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K546" s="1"/>
-    </row>
-    <row r="547" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K547" s="1"/>
-    </row>
-    <row r="548" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K548" s="1"/>
-    </row>
-    <row r="549" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K549" s="1"/>
-    </row>
-    <row r="550" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K550" s="1"/>
-    </row>
-    <row r="551" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K551" s="1"/>
-    </row>
-    <row r="552" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K552" s="1"/>
-    </row>
-    <row r="553" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K553" s="1"/>
-    </row>
-    <row r="554" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K554" s="1"/>
-    </row>
-    <row r="555" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K555" s="1"/>
-    </row>
-    <row r="556" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K556" s="1"/>
-    </row>
-    <row r="557" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K557" s="1"/>
-    </row>
-    <row r="558" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K558" s="1"/>
-    </row>
-    <row r="559" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K559" s="1"/>
-    </row>
-    <row r="560" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K560" s="1"/>
-    </row>
-    <row r="561" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K561" s="1"/>
-    </row>
-    <row r="562" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K562" s="1"/>
-    </row>
-    <row r="563" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K563" s="1"/>
-    </row>
-    <row r="564" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K564" s="1"/>
-    </row>
-    <row r="565" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K565" s="1"/>
-    </row>
-    <row r="566" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K566" s="1"/>
-    </row>
-    <row r="567" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K567" s="1"/>
-    </row>
-    <row r="568" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K568" s="1"/>
-    </row>
-    <row r="569" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K569" s="1"/>
-    </row>
-    <row r="570" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K570" s="1"/>
-    </row>
-    <row r="571" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K571" s="1"/>
-    </row>
-    <row r="572" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K572" s="1"/>
-    </row>
-    <row r="573" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K573" s="1"/>
-    </row>
-    <row r="574" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K574" s="1"/>
-    </row>
-    <row r="575" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K575" s="1"/>
-    </row>
-    <row r="576" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K576" s="1"/>
-    </row>
-    <row r="577" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K577" s="1"/>
-    </row>
-    <row r="578" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K578" s="1"/>
-    </row>
-    <row r="579" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K579" s="1"/>
-    </row>
-    <row r="580" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K580" s="1"/>
-    </row>
-    <row r="581" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K581" s="1"/>
-    </row>
-    <row r="582" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K582" s="1"/>
-    </row>
-    <row r="583" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K583" s="1"/>
-    </row>
-    <row r="584" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K584" s="1"/>
-    </row>
-    <row r="585" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K585" s="1"/>
-    </row>
-    <row r="586" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K586" s="1"/>
-    </row>
-    <row r="587" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K587" s="1"/>
-    </row>
-    <row r="588" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K588" s="1"/>
-    </row>
-    <row r="589" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K589" s="1"/>
-    </row>
-    <row r="590" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K590" s="1"/>
-    </row>
-    <row r="591" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K591" s="1"/>
-    </row>
-    <row r="592" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K592" s="1"/>
-    </row>
-    <row r="593" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K593" s="1"/>
-    </row>
-    <row r="594" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K594" s="1"/>
-    </row>
-    <row r="595" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K595" s="1"/>
-    </row>
-    <row r="596" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K596" s="1"/>
-    </row>
-    <row r="597" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K597" s="1"/>
-    </row>
-    <row r="598" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K598" s="1"/>
-    </row>
-    <row r="599" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K599" s="1"/>
-    </row>
-    <row r="600" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K600" s="1"/>
-    </row>
-    <row r="601" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="K601" s="1"/>
-    </row>
-    <row r="602" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J602">
-        <f t="shared" ref="J602:J609" si="2">LEN(I602)</f>
-        <v>0</v>
-      </c>
-      <c r="K602" s="1" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="603" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J603">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K603" s="1" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="604" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J604">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K604" s="1" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="605" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J605">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K605" s="1" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="606" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J606">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K606" s="1" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="607" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J607">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K607" s="1" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="608" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J608">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K608" s="1" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="609" spans="10:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="J609">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K609" s="1" t="s">
-        <v>1015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>